<commit_message>
Machine "funcionando". Falta el resto de las collections + shifts
</commit_message>
<xml_diff>
--- a/CMCP_Manufacturing/InputCMPC.xlsx
+++ b/CMCP_Manufacturing/InputCMPC.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ite02\Documents\Gaston\Source\CMPC-manufacturing\CMCP_Manufacturing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D72E07BF-F58A-4623-907E-AAC685D6A96A}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE06731F-0858-42BF-ABE2-7967AFA42972}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17940" windowHeight="6045" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17940" windowHeight="6045" tabRatio="500" firstSheet="1" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SKU" sheetId="4" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1272" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1297" uniqueCount="113">
   <si>
     <t>sku</t>
   </si>
@@ -297,6 +297,81 @@
   </si>
   <si>
     <t>days_on_hand</t>
+  </si>
+  <si>
+    <t>AR-1</t>
+  </si>
+  <si>
+    <t>AR-2</t>
+  </si>
+  <si>
+    <t>AR-3</t>
+  </si>
+  <si>
+    <t>AR-4</t>
+  </si>
+  <si>
+    <t>AR-5</t>
+  </si>
+  <si>
+    <t>BR-1</t>
+  </si>
+  <si>
+    <t>BR-2</t>
+  </si>
+  <si>
+    <t>BR-3</t>
+  </si>
+  <si>
+    <t>CH-1</t>
+  </si>
+  <si>
+    <t>CH-2</t>
+  </si>
+  <si>
+    <t>CH-3</t>
+  </si>
+  <si>
+    <t>CO-1</t>
+  </si>
+  <si>
+    <t>CO-2</t>
+  </si>
+  <si>
+    <t>EC-1</t>
+  </si>
+  <si>
+    <t>MX-1</t>
+  </si>
+  <si>
+    <t>MX-2</t>
+  </si>
+  <si>
+    <t>MX-3</t>
+  </si>
+  <si>
+    <t>MX-4</t>
+  </si>
+  <si>
+    <t>MX-5</t>
+  </si>
+  <si>
+    <t>MX-6</t>
+  </si>
+  <si>
+    <t>PE-1</t>
+  </si>
+  <si>
+    <t>PE-2</t>
+  </si>
+  <si>
+    <t>PE-3</t>
+  </si>
+  <si>
+    <t>UR-1</t>
+  </si>
+  <si>
+    <t>shifts</t>
   </si>
 </sst>
 </file>
@@ -1594,7 +1669,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:V277"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="8" ySplit="1" topLeftCell="O262" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="I1" sqref="I1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
@@ -21602,27 +21677,28 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="A1:N25"/>
+  <dimension ref="A1:O25"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="70" workbookViewId="0">
-      <selection activeCell="M1" sqref="M1:M1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="70" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2:D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="2" width="14.125" customWidth="1"/>
     <col min="3" max="3" width="11.625" customWidth="1"/>
-    <col min="4" max="4" width="22.125" customWidth="1"/>
-    <col min="5" max="5" width="23.375" customWidth="1"/>
-    <col min="6" max="6" width="21.875" customWidth="1"/>
-    <col min="7" max="7" width="23.125" customWidth="1"/>
-    <col min="8" max="8" width="22.125" customWidth="1"/>
-    <col min="9" max="9" width="21.375" customWidth="1"/>
-    <col min="10" max="10" width="21.625" customWidth="1"/>
-    <col min="11" max="11" width="21.375" customWidth="1"/>
+    <col min="4" max="4" width="11.625" style="8" customWidth="1"/>
+    <col min="5" max="5" width="22.125" customWidth="1"/>
+    <col min="6" max="6" width="23.375" customWidth="1"/>
+    <col min="7" max="7" width="21.875" customWidth="1"/>
+    <col min="8" max="8" width="23.125" customWidth="1"/>
+    <col min="9" max="9" width="22.125" customWidth="1"/>
+    <col min="10" max="10" width="21.375" customWidth="1"/>
+    <col min="11" max="11" width="21.625" customWidth="1"/>
+    <col min="12" max="12" width="21.375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>29</v>
       </c>
@@ -21632,43 +21708,46 @@
       <c r="C1" t="s">
         <v>47</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="8" t="s">
+        <v>112</v>
+      </c>
+      <c r="E1" t="s">
         <v>48</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>49</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>50</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>51</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>52</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>53</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>54</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>55</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>56</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>57</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>1</v>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>88</v>
       </c>
       <c r="B2">
         <v>450</v>
@@ -21676,43 +21755,46 @@
       <c r="C2">
         <v>1</v>
       </c>
-      <c r="D2">
+      <c r="D2" s="8">
+        <v>3</v>
+      </c>
+      <c r="E2">
         <v>9</v>
       </c>
-      <c r="E2">
+      <c r="F2">
         <v>49.620932307692293</v>
       </c>
-      <c r="F2">
+      <c r="G2">
         <v>2.8</v>
       </c>
-      <c r="G2">
+      <c r="H2">
         <v>73.3</v>
       </c>
-      <c r="H2">
+      <c r="I2">
         <v>81.478548846153828</v>
       </c>
-      <c r="I2">
+      <c r="J2">
         <v>287.3</v>
       </c>
-      <c r="J2">
+      <c r="K2">
         <v>9406</v>
       </c>
-      <c r="K2">
+      <c r="L2">
         <v>1456</v>
       </c>
-      <c r="L2">
+      <c r="M2">
         <v>-0.05</v>
       </c>
-      <c r="M2">
+      <c r="N2">
         <v>6</v>
       </c>
-      <c r="N2">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>2</v>
+      <c r="O2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>89</v>
       </c>
       <c r="B3">
         <v>450</v>
@@ -21720,43 +21802,46 @@
       <c r="C3">
         <v>1</v>
       </c>
-      <c r="D3">
+      <c r="D3" s="8">
+        <v>3</v>
+      </c>
+      <c r="E3">
         <v>9</v>
       </c>
-      <c r="E3">
+      <c r="F3">
         <v>49.620932307692293</v>
       </c>
-      <c r="F3">
+      <c r="G3">
         <v>2.8</v>
       </c>
-      <c r="G3">
+      <c r="H3">
         <v>73.3</v>
       </c>
-      <c r="H3">
+      <c r="I3">
         <v>81.478548846153828</v>
       </c>
-      <c r="I3">
+      <c r="J3">
         <v>284.60000000000002</v>
       </c>
-      <c r="J3">
+      <c r="K3">
         <v>8704</v>
       </c>
-      <c r="K3">
+      <c r="L3">
         <v>1500</v>
       </c>
-      <c r="L3">
+      <c r="M3">
         <v>-0.04</v>
       </c>
-      <c r="M3">
+      <c r="N3">
         <v>6</v>
       </c>
-      <c r="N3">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>3</v>
+      <c r="O3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>90</v>
       </c>
       <c r="B4">
         <v>500</v>
@@ -21764,43 +21849,46 @@
       <c r="C4">
         <v>1</v>
       </c>
-      <c r="D4">
+      <c r="D4" s="8">
+        <v>3</v>
+      </c>
+      <c r="E4">
         <v>8</v>
       </c>
-      <c r="E4">
+      <c r="F4">
         <v>49.620932307692293</v>
       </c>
-      <c r="F4">
+      <c r="G4">
         <v>2.8</v>
       </c>
-      <c r="G4">
+      <c r="H4">
         <v>73.3</v>
       </c>
-      <c r="H4">
+      <c r="I4">
         <v>75.275932307692287</v>
       </c>
-      <c r="I4">
+      <c r="J4">
         <v>323.5</v>
       </c>
-      <c r="J4">
+      <c r="K4">
         <v>9528</v>
       </c>
-      <c r="K4">
+      <c r="L4">
         <v>3760</v>
       </c>
-      <c r="L4">
+      <c r="M4">
         <v>-0.03</v>
       </c>
-      <c r="M4">
+      <c r="N4">
         <v>6</v>
       </c>
-      <c r="N4">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>4</v>
+      <c r="O4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>91</v>
       </c>
       <c r="B5">
         <v>600</v>
@@ -21808,43 +21896,46 @@
       <c r="C5">
         <v>1</v>
       </c>
-      <c r="D5">
+      <c r="D5" s="8">
+        <v>3</v>
+      </c>
+      <c r="E5">
         <v>8</v>
       </c>
-      <c r="E5">
+      <c r="F5">
         <v>49.620932307692293</v>
       </c>
-      <c r="F5">
+      <c r="G5">
         <v>2.8</v>
       </c>
-      <c r="G5">
+      <c r="H5">
         <v>73.3</v>
       </c>
-      <c r="H5">
+      <c r="I5">
         <v>75.275932307692287</v>
       </c>
-      <c r="I5">
+      <c r="J5">
         <v>376.9</v>
       </c>
-      <c r="J5">
+      <c r="K5">
         <v>10904</v>
       </c>
-      <c r="K5">
+      <c r="L5">
         <v>2463</v>
       </c>
-      <c r="L5">
+      <c r="M5">
         <v>-0.03</v>
       </c>
-      <c r="M5">
+      <c r="N5">
         <v>6</v>
       </c>
-      <c r="N5">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>5</v>
+      <c r="O5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>92</v>
       </c>
       <c r="B6">
         <v>800</v>
@@ -21852,43 +21943,46 @@
       <c r="C6">
         <v>1</v>
       </c>
-      <c r="D6">
+      <c r="D6" s="8">
+        <v>3</v>
+      </c>
+      <c r="E6">
         <v>9</v>
       </c>
-      <c r="E6">
+      <c r="F6">
         <v>49.620932307692293</v>
       </c>
-      <c r="F6">
+      <c r="G6">
         <v>2.8</v>
       </c>
-      <c r="G6">
+      <c r="H6">
         <v>73.3</v>
       </c>
-      <c r="H6">
+      <c r="I6">
         <v>81.478548846153828</v>
       </c>
-      <c r="I6">
+      <c r="J6">
         <v>387.8</v>
       </c>
-      <c r="J6">
+      <c r="K6">
         <v>12970</v>
       </c>
-      <c r="K6">
+      <c r="L6">
         <v>3468</v>
       </c>
-      <c r="L6">
-        <v>0</v>
-      </c>
       <c r="M6">
+        <v>0</v>
+      </c>
+      <c r="N6">
         <v>6</v>
       </c>
-      <c r="N6">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <v>1</v>
+      <c r="O6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>93</v>
       </c>
       <c r="B7">
         <v>500</v>
@@ -21896,43 +21990,46 @@
       <c r="C7">
         <v>2</v>
       </c>
-      <c r="D7">
+      <c r="D7" s="8">
+        <v>3</v>
+      </c>
+      <c r="E7">
         <v>7</v>
       </c>
-      <c r="E7">
+      <c r="F7">
         <v>74.963890226287916</v>
       </c>
-      <c r="F7">
+      <c r="G7">
         <v>0.8</v>
       </c>
-      <c r="G7">
+      <c r="H7">
         <v>99.551636976408275</v>
       </c>
-      <c r="H7">
+      <c r="I7">
         <v>75.548567645642748</v>
       </c>
-      <c r="I7">
+      <c r="J7">
         <v>221</v>
       </c>
-      <c r="J7">
+      <c r="K7">
         <v>6630</v>
       </c>
-      <c r="K7">
+      <c r="L7">
         <v>512.79999999999995</v>
       </c>
-      <c r="L7">
+      <c r="M7">
         <v>-4.07E-2</v>
       </c>
-      <c r="M7">
+      <c r="N7">
         <v>6</v>
       </c>
-      <c r="N7">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A8">
-        <v>2</v>
+      <c r="O7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>94</v>
       </c>
       <c r="B8">
         <v>500</v>
@@ -21940,43 +22037,46 @@
       <c r="C8">
         <v>2</v>
       </c>
-      <c r="D8">
+      <c r="D8" s="8">
+        <v>3</v>
+      </c>
+      <c r="E8">
         <v>7</v>
       </c>
-      <c r="E8">
+      <c r="F8">
         <v>74.963890226287916</v>
       </c>
-      <c r="F8">
+      <c r="G8">
         <v>0.8</v>
       </c>
-      <c r="G8">
+      <c r="H8">
         <v>99.551636976408275</v>
       </c>
-      <c r="H8">
+      <c r="I8">
         <v>75.548567645642748</v>
       </c>
-      <c r="I8">
+      <c r="J8">
         <v>221</v>
       </c>
-      <c r="J8">
+      <c r="K8">
         <v>6630</v>
       </c>
-      <c r="K8">
+      <c r="L8">
         <v>512.79999999999995</v>
       </c>
-      <c r="L8">
+      <c r="M8">
         <v>-5.0800000000000005E-2</v>
       </c>
-      <c r="M8">
+      <c r="N8">
         <v>6</v>
       </c>
-      <c r="N8">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A9">
-        <v>3</v>
+      <c r="O8">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>95</v>
       </c>
       <c r="B9">
         <v>700</v>
@@ -21984,43 +22084,46 @@
       <c r="C9">
         <v>2</v>
       </c>
-      <c r="D9">
+      <c r="D9" s="8">
+        <v>3</v>
+      </c>
+      <c r="E9">
         <v>8</v>
       </c>
-      <c r="E9">
+      <c r="F9">
         <v>71.235556090515161</v>
       </c>
-      <c r="F9">
+      <c r="G9">
         <v>0.8</v>
       </c>
-      <c r="G9">
+      <c r="H9">
         <v>99.551636976408275</v>
       </c>
-      <c r="H9">
+      <c r="I9">
         <v>81.190719788155988</v>
       </c>
-      <c r="I9">
+      <c r="J9">
         <v>221</v>
       </c>
-      <c r="J9">
+      <c r="K9">
         <v>6630</v>
       </c>
-      <c r="K9">
+      <c r="L9">
         <v>705.1</v>
       </c>
-      <c r="L9">
+      <c r="M9">
         <v>-4.1100000000000005E-2</v>
       </c>
-      <c r="M9">
+      <c r="N9">
         <v>6</v>
       </c>
-      <c r="N9">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A10">
-        <v>1</v>
+      <c r="O9">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>96</v>
       </c>
       <c r="B10">
         <v>400</v>
@@ -22028,43 +22131,46 @@
       <c r="C10">
         <v>3</v>
       </c>
-      <c r="D10">
+      <c r="D10" s="8">
+        <v>3</v>
+      </c>
+      <c r="E10">
         <v>6</v>
       </c>
-      <c r="E10">
+      <c r="F10">
         <v>61.53846153846154</v>
       </c>
-      <c r="F10">
-        <v>2</v>
-      </c>
       <c r="G10">
+        <v>2</v>
+      </c>
+      <c r="H10">
         <v>73.07692307692308</v>
       </c>
-      <c r="H10">
+      <c r="I10">
         <v>64.42307692307692</v>
       </c>
-      <c r="I10">
+      <c r="J10">
         <v>400</v>
       </c>
-      <c r="J10">
+      <c r="K10">
         <v>3333</v>
       </c>
-      <c r="K10">
+      <c r="L10">
         <v>1200</v>
       </c>
-      <c r="L10">
+      <c r="M10">
         <v>0.01</v>
       </c>
-      <c r="M10">
+      <c r="N10">
         <v>6</v>
       </c>
-      <c r="N10">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A11">
-        <v>2</v>
+      <c r="O10">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>97</v>
       </c>
       <c r="B11">
         <v>500</v>
@@ -22072,43 +22178,46 @@
       <c r="C11">
         <v>3</v>
       </c>
-      <c r="D11">
+      <c r="D11" s="8">
+        <v>3</v>
+      </c>
+      <c r="E11">
         <v>6</v>
       </c>
-      <c r="E11">
+      <c r="F11">
         <v>61.53846153846154</v>
       </c>
-      <c r="F11">
-        <v>2</v>
-      </c>
       <c r="G11">
+        <v>2</v>
+      </c>
+      <c r="H11">
         <v>73.07692307692308</v>
       </c>
-      <c r="H11">
+      <c r="I11">
         <v>64.42307692307692</v>
       </c>
-      <c r="I11">
+      <c r="J11">
         <v>533.33333333333337</v>
       </c>
-      <c r="J11">
+      <c r="K11">
         <v>3333</v>
       </c>
-      <c r="K11">
+      <c r="L11">
         <v>1200</v>
       </c>
-      <c r="L11">
+      <c r="M11">
         <v>0.01</v>
       </c>
-      <c r="M11">
+      <c r="N11">
         <v>6</v>
       </c>
-      <c r="N11">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A12">
-        <v>3</v>
+      <c r="O11">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>98</v>
       </c>
       <c r="B12">
         <v>800</v>
@@ -22116,43 +22225,46 @@
       <c r="C12">
         <v>3</v>
       </c>
-      <c r="D12">
+      <c r="D12" s="8">
+        <v>3</v>
+      </c>
+      <c r="E12">
         <v>7</v>
       </c>
-      <c r="E12">
+      <c r="F12">
         <v>61.53846153846154</v>
       </c>
-      <c r="F12">
-        <v>2</v>
-      </c>
       <c r="G12">
+        <v>2</v>
+      </c>
+      <c r="H12">
         <v>73.07692307692308</v>
       </c>
-      <c r="H12">
+      <c r="I12">
         <v>72.115384615384613</v>
       </c>
-      <c r="I12">
+      <c r="J12">
         <v>533.33333333333337</v>
       </c>
-      <c r="J12">
+      <c r="K12">
         <v>3333</v>
       </c>
-      <c r="K12">
+      <c r="L12">
         <v>1200</v>
       </c>
-      <c r="L12">
+      <c r="M12">
         <v>0.01</v>
       </c>
-      <c r="M12">
+      <c r="N12">
         <v>6</v>
       </c>
-      <c r="N12">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A13">
-        <v>1</v>
+      <c r="O12">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>99</v>
       </c>
       <c r="B13">
         <v>350</v>
@@ -22160,43 +22272,46 @@
       <c r="C13">
         <v>4</v>
       </c>
-      <c r="D13">
+      <c r="D13" s="8">
+        <v>3</v>
+      </c>
+      <c r="E13">
         <v>8</v>
       </c>
-      <c r="E13">
+      <c r="F13">
         <v>28.53846153846154</v>
       </c>
-      <c r="F13">
-        <v>2</v>
-      </c>
       <c r="G13">
+        <v>2</v>
+      </c>
+      <c r="H13">
         <v>40</v>
       </c>
-      <c r="H13">
+      <c r="I13">
         <v>38.53846153846154</v>
       </c>
-      <c r="I13">
+      <c r="J13">
         <v>114.2</v>
       </c>
-      <c r="J13">
+      <c r="K13">
         <v>9406</v>
       </c>
-      <c r="K13">
+      <c r="L13">
         <v>1456</v>
       </c>
-      <c r="L13">
+      <c r="M13">
         <v>-0.05</v>
       </c>
-      <c r="M13">
+      <c r="N13">
         <v>6</v>
       </c>
-      <c r="N13">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A14">
-        <v>2</v>
+      <c r="O13">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>100</v>
       </c>
       <c r="B14">
         <v>420</v>
@@ -22204,43 +22319,46 @@
       <c r="C14">
         <v>4</v>
       </c>
-      <c r="D14">
+      <c r="D14" s="8">
+        <v>3</v>
+      </c>
+      <c r="E14">
         <v>9</v>
       </c>
-      <c r="E14">
+      <c r="F14">
         <v>35.67307692307692</v>
       </c>
-      <c r="F14">
-        <v>2</v>
-      </c>
       <c r="G14">
+        <v>2</v>
+      </c>
+      <c r="H14">
         <v>40</v>
       </c>
-      <c r="H14">
+      <c r="I14">
         <v>50.132211538461533</v>
       </c>
-      <c r="I14">
+      <c r="J14">
         <v>284.60000000000002</v>
       </c>
-      <c r="J14">
+      <c r="K14">
         <v>8704</v>
       </c>
-      <c r="K14">
+      <c r="L14">
         <v>1500</v>
       </c>
-      <c r="L14">
+      <c r="M14">
         <v>-0.04</v>
       </c>
-      <c r="M14">
+      <c r="N14">
         <v>6</v>
       </c>
-      <c r="N14">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A15">
-        <v>1</v>
+      <c r="O14">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>101</v>
       </c>
       <c r="B15">
         <v>600</v>
@@ -22248,43 +22366,46 @@
       <c r="C15">
         <v>5</v>
       </c>
-      <c r="D15">
+      <c r="D15" s="8">
+        <v>3</v>
+      </c>
+      <c r="E15">
         <v>9</v>
       </c>
-      <c r="E15">
+      <c r="F15">
         <v>60</v>
       </c>
-      <c r="F15">
+      <c r="G15">
         <v>7</v>
       </c>
-      <c r="G15">
+      <c r="H15">
         <v>82.142857142857139</v>
       </c>
-      <c r="H15">
+      <c r="I15">
         <v>139.375</v>
       </c>
-      <c r="I15">
+      <c r="J15">
         <v>197.2222222222222</v>
       </c>
-      <c r="J15">
+      <c r="K15">
         <v>7000</v>
       </c>
-      <c r="K15">
+      <c r="L15">
         <v>1000</v>
       </c>
-      <c r="L15">
+      <c r="M15">
         <v>9.999999999999995E-3</v>
       </c>
-      <c r="M15">
+      <c r="N15">
         <v>6</v>
       </c>
-      <c r="N15">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A16">
-        <v>1</v>
+      <c r="O15">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>102</v>
       </c>
       <c r="B16">
         <v>400</v>
@@ -22292,43 +22413,46 @@
       <c r="C16">
         <v>6</v>
       </c>
-      <c r="D16">
+      <c r="D16" s="8">
+        <v>3</v>
+      </c>
+      <c r="E16">
         <v>8</v>
       </c>
-      <c r="E16">
+      <c r="F16">
         <v>32.94</v>
       </c>
-      <c r="F16">
-        <v>2</v>
-      </c>
       <c r="G16">
+        <v>2</v>
+      </c>
+      <c r="H16">
         <v>65.3</v>
       </c>
-      <c r="H16">
+      <c r="I16">
         <v>49.265000000000001</v>
       </c>
-      <c r="I16">
+      <c r="J16">
         <v>212</v>
       </c>
-      <c r="J16">
+      <c r="K16">
         <v>6486</v>
       </c>
-      <c r="K16">
+      <c r="L16">
         <v>1000</v>
       </c>
-      <c r="L16">
-        <v>0</v>
-      </c>
       <c r="M16">
+        <v>0</v>
+      </c>
+      <c r="N16">
         <v>6</v>
       </c>
-      <c r="N16">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A17">
-        <v>2</v>
+      <c r="O16">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>103</v>
       </c>
       <c r="B17">
         <v>360</v>
@@ -22336,43 +22460,46 @@
       <c r="C17">
         <v>6</v>
       </c>
-      <c r="D17">
+      <c r="D17" s="8">
+        <v>3</v>
+      </c>
+      <c r="E17">
         <v>8</v>
       </c>
-      <c r="E17">
+      <c r="F17">
         <v>32.94</v>
       </c>
-      <c r="F17">
-        <v>2</v>
-      </c>
       <c r="G17">
+        <v>2</v>
+      </c>
+      <c r="H17">
         <v>65.3</v>
       </c>
-      <c r="H17">
+      <c r="I17">
         <v>49.265000000000001</v>
       </c>
-      <c r="I17">
+      <c r="J17">
         <v>164</v>
       </c>
-      <c r="J17">
+      <c r="K17">
         <v>6486</v>
       </c>
-      <c r="K17">
+      <c r="L17">
         <v>1000</v>
       </c>
-      <c r="L17">
-        <v>0</v>
-      </c>
       <c r="M17">
+        <v>0</v>
+      </c>
+      <c r="N17">
         <v>6</v>
       </c>
-      <c r="N17">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A18">
-        <v>3</v>
+      <c r="O17">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>104</v>
       </c>
       <c r="B18">
         <v>360</v>
@@ -22380,43 +22507,46 @@
       <c r="C18">
         <v>6</v>
       </c>
-      <c r="D18">
+      <c r="D18" s="8">
+        <v>3</v>
+      </c>
+      <c r="E18">
         <v>8</v>
       </c>
-      <c r="E18">
+      <c r="F18">
         <v>32.94</v>
       </c>
-      <c r="F18">
-        <v>2</v>
-      </c>
       <c r="G18">
+        <v>2</v>
+      </c>
+      <c r="H18">
         <v>65.3</v>
       </c>
-      <c r="H18">
+      <c r="I18">
         <v>49.265000000000001</v>
       </c>
-      <c r="I18">
+      <c r="J18">
         <v>205</v>
       </c>
-      <c r="J18">
+      <c r="K18">
         <v>6486</v>
       </c>
-      <c r="K18">
+      <c r="L18">
         <v>1000</v>
       </c>
-      <c r="L18">
-        <v>0</v>
-      </c>
       <c r="M18">
+        <v>0</v>
+      </c>
+      <c r="N18">
         <v>6</v>
       </c>
-      <c r="N18">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A19">
-        <v>4</v>
+      <c r="O18">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>105</v>
       </c>
       <c r="B19">
         <v>500</v>
@@ -22424,43 +22554,46 @@
       <c r="C19">
         <v>6</v>
       </c>
-      <c r="D19">
+      <c r="D19" s="8">
+        <v>3</v>
+      </c>
+      <c r="E19">
         <v>8</v>
       </c>
-      <c r="E19">
+      <c r="F19">
         <v>32.94</v>
       </c>
-      <c r="F19">
-        <v>2</v>
-      </c>
       <c r="G19">
+        <v>2</v>
+      </c>
+      <c r="H19">
         <v>65.3</v>
       </c>
-      <c r="H19">
+      <c r="I19">
         <v>49.265000000000001</v>
       </c>
-      <c r="I19">
+      <c r="J19">
         <v>222</v>
       </c>
-      <c r="J19">
+      <c r="K19">
         <v>6486</v>
       </c>
-      <c r="K19">
+      <c r="L19">
         <v>1000</v>
       </c>
-      <c r="L19">
-        <v>0</v>
-      </c>
       <c r="M19">
+        <v>0</v>
+      </c>
+      <c r="N19">
         <v>6</v>
       </c>
-      <c r="N19">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A20">
-        <v>5</v>
+      <c r="O19">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>106</v>
       </c>
       <c r="B20">
         <v>600</v>
@@ -22468,43 +22601,46 @@
       <c r="C20">
         <v>6</v>
       </c>
-      <c r="D20">
+      <c r="D20" s="8">
+        <v>3</v>
+      </c>
+      <c r="E20">
         <v>8</v>
       </c>
-      <c r="E20">
+      <c r="F20">
         <v>32.94</v>
       </c>
-      <c r="F20">
+      <c r="G20">
         <v>3</v>
       </c>
-      <c r="G20">
+      <c r="H20">
         <v>65.3</v>
       </c>
-      <c r="H20">
+      <c r="I20">
         <v>57.427499999999995</v>
       </c>
-      <c r="I20">
+      <c r="J20">
         <v>243</v>
       </c>
-      <c r="J20">
+      <c r="K20">
         <v>6486</v>
       </c>
-      <c r="K20">
+      <c r="L20">
         <v>1000</v>
       </c>
-      <c r="L20">
+      <c r="M20">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="M20">
+      <c r="N20">
         <v>6</v>
       </c>
-      <c r="N20">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A21">
-        <v>6</v>
+      <c r="O20">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>107</v>
       </c>
       <c r="B21">
         <v>800</v>
@@ -22512,43 +22648,46 @@
       <c r="C21">
         <v>6</v>
       </c>
-      <c r="D21">
+      <c r="D21" s="8">
+        <v>3</v>
+      </c>
+      <c r="E21">
         <v>8</v>
       </c>
-      <c r="E21">
+      <c r="F21">
         <v>32.94</v>
       </c>
-      <c r="F21">
+      <c r="G21">
         <v>3</v>
       </c>
-      <c r="G21">
+      <c r="H21">
         <v>65.3</v>
       </c>
-      <c r="H21">
+      <c r="I21">
         <v>57.427499999999995</v>
       </c>
-      <c r="I21">
+      <c r="J21">
         <v>243</v>
       </c>
-      <c r="J21">
+      <c r="K21">
         <v>6486</v>
       </c>
-      <c r="K21">
+      <c r="L21">
         <v>1000</v>
       </c>
-      <c r="L21">
+      <c r="M21">
         <v>0.01</v>
       </c>
-      <c r="M21">
+      <c r="N21">
         <v>6</v>
       </c>
-      <c r="N21">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A22">
-        <v>1</v>
+      <c r="O21">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>108</v>
       </c>
       <c r="B22">
         <v>400</v>
@@ -22556,43 +22695,46 @@
       <c r="C22">
         <v>7</v>
       </c>
-      <c r="D22">
+      <c r="D22" s="8">
+        <v>3</v>
+      </c>
+      <c r="E22">
         <v>6</v>
       </c>
-      <c r="E22">
+      <c r="F22">
         <v>31.401452028889345</v>
       </c>
-      <c r="F22">
+      <c r="G22">
         <v>3.2222222222222223</v>
       </c>
-      <c r="G22">
+      <c r="H22">
         <v>81.17242004738128</v>
       </c>
-      <c r="H22">
+      <c r="I22">
         <v>56.245535985195581</v>
       </c>
-      <c r="I22">
+      <c r="J22">
         <v>232.3457962962963</v>
       </c>
-      <c r="J22">
+      <c r="K22">
         <v>3271.4175732133326</v>
       </c>
-      <c r="K22">
+      <c r="L22">
         <v>460.15885128205127</v>
       </c>
-      <c r="L22">
+      <c r="M22">
         <v>-1.9188498652814037E-2</v>
       </c>
-      <c r="M22">
+      <c r="N22">
         <v>6</v>
       </c>
-      <c r="N22">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A23">
-        <v>2</v>
+      <c r="O22">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>109</v>
       </c>
       <c r="B23">
         <v>500</v>
@@ -22600,43 +22742,46 @@
       <c r="C23">
         <v>7</v>
       </c>
-      <c r="D23">
+      <c r="D23" s="8">
+        <v>3</v>
+      </c>
+      <c r="E23">
         <v>6</v>
       </c>
-      <c r="E23">
+      <c r="F23">
         <v>31.401452028889345</v>
       </c>
-      <c r="F23">
+      <c r="G23">
         <v>3.2222222222222223</v>
       </c>
-      <c r="G23">
+      <c r="H23">
         <v>81.17242004738128</v>
       </c>
-      <c r="H23">
+      <c r="I23">
         <v>56.245535985195581</v>
       </c>
-      <c r="I23">
+      <c r="J23">
         <v>241.3935185185185</v>
       </c>
-      <c r="J23">
+      <c r="K23">
         <v>3271.4175732133326</v>
       </c>
-      <c r="K23">
+      <c r="L23">
         <v>659.40738461538467</v>
       </c>
-      <c r="L23">
+      <c r="M23">
         <v>-1.9424940820560108E-2</v>
       </c>
-      <c r="M23">
+      <c r="N23">
         <v>6</v>
       </c>
-      <c r="N23">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A24">
-        <v>3</v>
+      <c r="O23">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>110</v>
       </c>
       <c r="B24">
         <v>500</v>
@@ -22644,43 +22789,46 @@
       <c r="C24">
         <v>7</v>
       </c>
-      <c r="D24">
+      <c r="D24" s="8">
+        <v>3</v>
+      </c>
+      <c r="E24">
         <v>7</v>
       </c>
-      <c r="E24">
+      <c r="F24">
         <v>31.401452028889345</v>
       </c>
-      <c r="F24">
+      <c r="G24">
         <v>3.2222222222222223</v>
       </c>
-      <c r="G24">
+      <c r="H24">
         <v>81.17242004738128</v>
       </c>
-      <c r="H24">
+      <c r="I24">
         <v>60.170717488806744</v>
       </c>
-      <c r="I24">
+      <c r="J24">
         <v>234.09348148148149</v>
       </c>
-      <c r="J24">
+      <c r="K24">
         <v>3271.4175732133326</v>
       </c>
-      <c r="K24">
+      <c r="L24">
         <v>1138.0806017094017</v>
       </c>
-      <c r="L24">
+      <c r="M24">
         <v>-5.6073892456998467E-3</v>
       </c>
-      <c r="M24">
+      <c r="N24">
         <v>6</v>
       </c>
-      <c r="N24">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A25">
-        <v>1</v>
+      <c r="O24">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>111</v>
       </c>
       <c r="B25">
         <v>600</v>
@@ -22688,37 +22836,40 @@
       <c r="C25">
         <v>8</v>
       </c>
-      <c r="D25">
+      <c r="D25" s="8">
+        <v>3</v>
+      </c>
+      <c r="E25">
         <v>7</v>
       </c>
-      <c r="E25">
+      <c r="F25">
         <v>32.051282051282051</v>
       </c>
-      <c r="F25">
+      <c r="G25">
         <v>5</v>
       </c>
-      <c r="G25">
+      <c r="H25">
         <v>38.4</v>
       </c>
-      <c r="H25">
+      <c r="I25">
         <v>52.044871794871796</v>
       </c>
-      <c r="I25">
+      <c r="J25">
         <v>256.41025641025641</v>
       </c>
-      <c r="J25">
+      <c r="K25">
         <v>7000</v>
       </c>
-      <c r="K25">
+      <c r="L25">
         <v>1260</v>
       </c>
-      <c r="L25">
+      <c r="M25">
         <v>3.9999999999999994E-2</v>
       </c>
-      <c r="M25">
+      <c r="N25">
         <v>6</v>
       </c>
-      <c r="N25">
+      <c r="O25">
         <v>2</v>
       </c>
     </row>

</xml_diff>